<commit_message>
Add gem file lock
</commit_message>
<xml_diff>
--- a/files/templates/transaction.xlsx
+++ b/files/templates/transaction.xlsx
@@ -286,22 +286,23 @@
   </sheetPr>
   <dimension ref="B1:K5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L3" activeCellId="0" sqref="L3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="5.57085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="7.49797570850202"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.8542510121457"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="46.7044534412956"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="28.9230769230769"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="17.7813765182186"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="20.1740890688259"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="1" width="18.7368421052632"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="3.63562753036437"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="6.49797570850202"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.4331983805668"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.1902834008097"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="43.1052631578947"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="27.1214574898785"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="15.8744939271255"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.6923076923077"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="18.9595141700405"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="17.417004048583"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="17.8582995951417"/>
     <col collapsed="false" hidden="false" max="1018" min="12" style="1" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1025" min="1019" style="0" width="9.10526315789474"/>
   </cols>

</xml_diff>

<commit_message>
Create selectbox excel and sheet master
</commit_message>
<xml_diff>
--- a/files/templates/transaction.xlsx
+++ b/files/templates/transaction.xlsx
@@ -9,6 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="Transaction" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Master" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t xml:space="preserve">TRANSACTION REPORT</t>
   </si>
@@ -50,6 +51,21 @@
   </si>
   <si>
     <t xml:space="preserve">SAVED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GROUP MEMBER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRANSACTION TYPE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EMAIL</t>
   </si>
 </sst>
 </file>
@@ -59,7 +75,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -105,8 +121,23 @@
       <family val="1"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -116,13 +147,25 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
-        <bgColor rgb="FF008080"/>
+        <bgColor rgb="FF00CC33"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF33FF"/>
         <bgColor rgb="FFFF00FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00CC33"/>
+        <bgColor rgb="FF00B050"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFF00"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -174,7 +217,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -205,6 +248,22 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -221,9 +280,9 @@
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
       <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF00CC33"/>
       <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFCCFF00"/>
       <rgbColor rgb="FFFF33FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
@@ -287,22 +346,22 @@
   <dimension ref="B1:K5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="3.63562753036437"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="6.49797570850202"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.4331983805668"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.1902834008097"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="43.1052631578947"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="27.1214574898785"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="15.8744939271255"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.6923076923077"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="18.9595141700405"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="17.417004048583"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="17.8582995951417"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="3.64372469635628"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="6.42914979757085"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.6396761133603"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.4251012145749"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="43.8097165991903"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="27.5303643724696"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="16.0688259109312"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.7125506072875"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="19.3886639676113"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="17.6761133603239"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="18.1012145748988"/>
     <col collapsed="false" hidden="false" max="1018" min="12" style="1" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1025" min="1019" style="0" width="9.10526315789474"/>
   </cols>
@@ -385,4 +444,84 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="B1:H65536"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H12" activeCellId="0" sqref="H12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="4.2834008097166"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="8" width="7.92712550607287"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="8" width="26.1376518218623"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="8" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="8" width="7.92712550607287"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="8" width="19.2834008097166"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="8" width="9.10526315789474"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="0"/>
+      <c r="C1" s="0"/>
+      <c r="D1" s="0"/>
+      <c r="G1" s="0"/>
+      <c r="H1" s="0"/>
+    </row>
+    <row r="2" customFormat="false" ht="23.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B2" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="G2" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="9"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="0"/>
+      <c r="C3" s="0"/>
+      <c r="D3" s="0"/>
+      <c r="G3" s="0"/>
+      <c r="H3" s="0"/>
+    </row>
+    <row r="4" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B4" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="G2:H2"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>